<commit_message>
Generate XML Database Function Finish
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Excel/AVCARDDB.xlsx
+++ b/Assets/StreamingAssets/Excel/AVCARDDB.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11900" yWindow="360" windowWidth="29360" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="11895" yWindow="420" windowWidth="29040" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Starter1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>CardNo</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,167 +85,171 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>PG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学級委員である文がいるだけで、何故かクラスがまとまるのだ。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超能力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVST1/B1-006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1-007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ゲーマー少女　琴吹文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Illustrator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>七</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>七</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{[自動型能力,リンク‐リンクステップ開始時［リンク6‐①ΣΩ］ そのターン中、このカードのパワーを＋5000。]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文の目には何でも見えている。敵の動きも……弱点でさえも。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVST1/B1-007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1-008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全国ランカー　琴吹文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{[自動型能力,リンク‐リンクステップ開始時［リンク7‐①ΣΩ］ そのターン中、このカードのパワーを＋4000。]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>「確かに私の目はよく見えるけど、見えるのと動けるのは違うよ」</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVST1/B1-008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1-009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>後輩　佐久良舞衣菜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIGUMA*1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{[起動型能力,(FALL)あなたの山札の上を見て、山札の上か捨札に置く。]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>「先輩っ！」見つめる舞衣菜の瞳には、夢と希望が輝いている。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一葉モカ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVST1/B1-009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1-016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陸上部　土屋原はねる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{[自動型能力,リンク‐リンクステップ開始時［リンク5‐②Σ］ そのターン中、このカードのパワーを＋6000。]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>「アスリートだからね！」はねるはそう言うと、人懐っこく笑う。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ニリツ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVST1/B1-016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>学級委員　琴吹文</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>青</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学級委員である文がいるだけで、何故かクラスがまとまるのだ。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>人間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>超能力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVST1/B1-006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B1-007</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ゲーマー少女　琴吹文</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Illustrator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>七</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>七</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{[自動型能力,リンク‐リンクステップ開始時［リンク6‐①ΣΩ］ そのターン中、このカードのパワーを＋5000。]}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文の目には何でも見えている。敵の動きも……弱点でさえも。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVST1/B1-007</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B1-008</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>全国ランカー　琴吹文</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{[自動型能力,リンク‐リンクステップ開始時［リンク7‐①ΣΩ］ そのターン中、このカードのパワーを＋4000。]}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>「確かに私の目はよく見えるけど、見えるのと動けるのは違うよ」</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVST1/B1-008</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B1-009</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rare</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>U</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>後輩　佐久良舞衣菜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SIGUMA*1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{[起動型能力,(FALL)あなたの山札の上を見て、山札の上か捨札に置く。]}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>「先輩っ！」見つめる舞衣菜の瞳には、夢と希望が輝いている。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一葉モカ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVST1/B1-009</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B1-016</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>陸上部　土屋原はねる</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{[自動型能力,リンク‐リンクステップ開始時［リンク5‐②Σ］ そのターン中、このカードのパワーを＋6000。]}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>「アスリートだからね！」はねるはそう言うと、人懐っこく笑う。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ニリツ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVST1/B1-016</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -346,24 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="35">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -381,9 +368,31 @@
     <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -712,20 +721,20 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+    <col min="9" max="9" width="18.125" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -772,42 +781,42 @@
         <v>13</v>
       </c>
       <c r="P1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
       </c>
       <c r="K2">
         <v>5000</v>
@@ -816,51 +825,51 @@
         <v>4000</v>
       </c>
       <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
         <v>22</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
       </c>
       <c r="O2">
         <v>2</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
         <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
       </c>
       <c r="K3">
         <v>8000</v>
@@ -869,51 +878,51 @@
         <v>4000</v>
       </c>
       <c r="M3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" t="s">
         <v>22</v>
-      </c>
-      <c r="N3" t="s">
-        <v>23</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
         <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
       </c>
       <c r="K4">
         <v>10000</v>
@@ -922,51 +931,51 @@
         <v>4000</v>
       </c>
       <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
         <v>22</v>
-      </c>
-      <c r="N4" t="s">
-        <v>23</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
         <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
         <v>46</v>
-      </c>
-      <c r="J5" t="s">
-        <v>47</v>
       </c>
       <c r="K5">
         <v>6000</v>
@@ -975,51 +984,51 @@
         <v>4000</v>
       </c>
       <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
         <v>22</v>
-      </c>
-      <c r="N5" t="s">
-        <v>23</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q5" t="s">
         <v>48</v>
       </c>
-      <c r="Q5" t="s">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
         <v>53</v>
-      </c>
-      <c r="J6" t="s">
-        <v>54</v>
       </c>
       <c r="K6">
         <v>6000</v>
@@ -1028,19 +1037,19 @@
         <v>4000</v>
       </c>
       <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" t="s">
         <v>22</v>
-      </c>
-      <c r="N6" t="s">
-        <v>23</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6" t="s">
         <v>55</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>